<commit_message>
updated documents for updated sections implementation
</commit_message>
<xml_diff>
--- a/docs/distrib_nested.xlsx
+++ b/docs/distrib_nested.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\learning\distributed\OpenMP Codon Frequency\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9169E34-8535-47A5-B808-6AC6C11C1791}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4A3D3C9-248A-478B-8172-9798FAF02470}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10540" xr2:uid="{4E395B02-0435-48AB-AD0A-878D34393581}"/>
   </bookViews>
@@ -209,16 +209,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>413</c:v>
+                  <c:v>205</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>405</c:v>
+                  <c:v>172</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>430</c:v>
+                  <c:v>178</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>463</c:v>
+                  <c:v>179</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -296,16 +296,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>346</c:v>
+                  <c:v>169</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>207</c:v>
+                  <c:v>113</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>217</c:v>
+                  <c:v>123</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>251</c:v>
+                  <c:v>155</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1518,8 +1518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A53BF75-6442-4B9C-A0A6-243CF8E8CACB}">
   <dimension ref="A2:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1563,18 +1563,18 @@
         <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>546</v>
+        <v>337</v>
       </c>
       <c r="C4" s="1">
-        <v>346</v>
+        <v>169</v>
       </c>
       <c r="D4" s="2">
         <f>B4/C4</f>
-        <v>1.5780346820809248</v>
+        <v>1.9940828402366864</v>
       </c>
       <c r="E4" s="1">
         <f>D4/A4</f>
-        <v>0.78901734104046239</v>
+        <v>0.99704142011834318</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
@@ -1582,18 +1582,18 @@
         <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>492</v>
+        <v>255</v>
       </c>
       <c r="C5" s="1">
-        <v>207</v>
+        <v>113</v>
       </c>
       <c r="D5" s="2">
         <f t="shared" ref="D5:D7" si="0">B5/C5</f>
-        <v>2.3768115942028984</v>
+        <v>2.2566371681415931</v>
       </c>
       <c r="E5" s="1">
         <f t="shared" ref="E5:E7" si="1">D5/A5</f>
-        <v>0.59420289855072461</v>
+        <v>0.56415929203539827</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -1601,18 +1601,18 @@
         <v>8</v>
       </c>
       <c r="B6" s="1">
-        <v>470</v>
+        <v>232</v>
       </c>
       <c r="C6" s="1">
-        <v>217</v>
+        <v>123</v>
       </c>
       <c r="D6" s="2">
         <f t="shared" si="0"/>
-        <v>2.1658986175115209</v>
+        <v>1.8861788617886179</v>
       </c>
       <c r="E6" s="1">
         <f t="shared" si="1"/>
-        <v>0.27073732718894011</v>
+        <v>0.23577235772357724</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
@@ -1620,18 +1620,18 @@
         <v>16</v>
       </c>
       <c r="B7" s="1">
-        <v>474</v>
+        <v>229</v>
       </c>
       <c r="C7" s="1">
-        <v>251</v>
+        <v>155</v>
       </c>
       <c r="D7" s="2">
         <f t="shared" si="0"/>
-        <v>1.8884462151394423</v>
+        <v>1.4774193548387098</v>
       </c>
       <c r="E7" s="1">
         <f t="shared" si="1"/>
-        <v>0.11802788844621515</v>
+        <v>9.2338709677419362E-2</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
@@ -1644,19 +1644,19 @@
       </c>
       <c r="B9" s="2">
         <f>SUM(B4:B7)/4</f>
-        <v>495.5</v>
+        <v>263.25</v>
       </c>
       <c r="C9" s="2">
         <f>SUM(C4:C7)/4</f>
-        <v>255.25</v>
+        <v>140</v>
       </c>
       <c r="D9" s="2">
         <f>SUM(D4:D7)/4</f>
-        <v>2.0022977772336965</v>
+        <v>1.9035795562514017</v>
       </c>
       <c r="E9" s="1">
         <f>SUM(E4:E7)/4</f>
-        <v>0.44299636380658558</v>
+        <v>0.47232794488868451</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="29" x14ac:dyDescent="0.35">
@@ -1689,18 +1689,18 @@
         <v>2</v>
       </c>
       <c r="B14" s="1">
-        <v>546</v>
+        <v>337</v>
       </c>
       <c r="C14" s="1">
-        <v>413</v>
+        <v>205</v>
       </c>
       <c r="D14" s="2">
         <f>B14/C14</f>
-        <v>1.3220338983050848</v>
+        <v>1.6439024390243901</v>
       </c>
       <c r="E14" s="1">
         <f>D14/A14</f>
-        <v>0.66101694915254239</v>
+        <v>0.82195121951219507</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
@@ -1708,18 +1708,18 @@
         <v>4</v>
       </c>
       <c r="B15" s="1">
-        <v>492</v>
+        <v>255</v>
       </c>
       <c r="C15" s="1">
-        <v>405</v>
+        <v>172</v>
       </c>
       <c r="D15" s="2">
         <f t="shared" ref="D15:D17" si="2">B15/C15</f>
-        <v>1.2148148148148148</v>
+        <v>1.4825581395348837</v>
       </c>
       <c r="E15" s="1">
         <f t="shared" ref="E15:E17" si="3">D15/A15</f>
-        <v>0.3037037037037037</v>
+        <v>0.37063953488372092</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
@@ -1727,18 +1727,18 @@
         <v>8</v>
       </c>
       <c r="B16" s="1">
-        <v>470</v>
+        <v>232</v>
       </c>
       <c r="C16" s="1">
-        <v>430</v>
+        <v>178</v>
       </c>
       <c r="D16" s="2">
         <f t="shared" si="2"/>
-        <v>1.0930232558139534</v>
+        <v>1.303370786516854</v>
       </c>
       <c r="E16" s="1">
         <f t="shared" si="3"/>
-        <v>0.13662790697674418</v>
+        <v>0.16292134831460675</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
@@ -1746,18 +1746,18 @@
         <v>16</v>
       </c>
       <c r="B17" s="1">
-        <v>474</v>
+        <v>229</v>
       </c>
       <c r="C17" s="1">
-        <v>463</v>
+        <v>179</v>
       </c>
       <c r="D17" s="2">
         <f t="shared" si="2"/>
-        <v>1.0237580993520519</v>
+        <v>1.2793296089385475</v>
       </c>
       <c r="E17" s="1">
         <f t="shared" si="3"/>
-        <v>6.3984881209503242E-2</v>
+        <v>7.995810055865922E-2</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
@@ -1770,19 +1770,19 @@
       </c>
       <c r="B19" s="2">
         <f>SUM(B14:B17)/4</f>
-        <v>495.5</v>
+        <v>263.25</v>
       </c>
       <c r="C19" s="2">
         <f>SUM(C14:C17)/4</f>
-        <v>427.75</v>
+        <v>183.5</v>
       </c>
       <c r="D19" s="2">
         <f>SUM(D14:D17)/4</f>
-        <v>1.1634075170714762</v>
+        <v>1.4272902435036687</v>
       </c>
       <c r="E19" s="1">
         <f>SUM(E14:E17)/4</f>
-        <v>0.29133336026062334</v>
+        <v>0.35886755081729549</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -1809,13 +1809,13 @@
         <v>2</v>
       </c>
       <c r="B24" s="1">
-        <v>546</v>
+        <v>337</v>
       </c>
       <c r="C24" s="1">
-        <v>413</v>
+        <v>205</v>
       </c>
       <c r="D24" s="1">
-        <v>346</v>
+        <v>169</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
@@ -1823,13 +1823,13 @@
         <v>4</v>
       </c>
       <c r="B25" s="1">
-        <v>492</v>
+        <v>255</v>
       </c>
       <c r="C25" s="1">
-        <v>405</v>
+        <v>172</v>
       </c>
       <c r="D25" s="1">
-        <v>207</v>
+        <v>113</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
@@ -1837,13 +1837,13 @@
         <v>8</v>
       </c>
       <c r="B26" s="1">
-        <v>470</v>
+        <v>232</v>
       </c>
       <c r="C26" s="1">
-        <v>430</v>
+        <v>178</v>
       </c>
       <c r="D26" s="1">
-        <v>217</v>
+        <v>123</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
@@ -1851,13 +1851,13 @@
         <v>16</v>
       </c>
       <c r="B27" s="1">
-        <v>474</v>
+        <v>229</v>
       </c>
       <c r="C27" s="1">
-        <v>463</v>
+        <v>179</v>
       </c>
       <c r="D27" s="1">
-        <v>251</v>
+        <v>155</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
@@ -1866,15 +1866,15 @@
       </c>
       <c r="B29" s="2">
         <f>SUM(B24:B27)/4</f>
-        <v>495.5</v>
+        <v>263.25</v>
       </c>
       <c r="C29" s="2">
         <f>SUM(C24:C27)/4</f>
-        <v>427.75</v>
+        <v>183.5</v>
       </c>
       <c r="D29" s="2">
         <f>SUM(D24:D27)/4</f>
-        <v>255.25</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>

</xml_diff>